<commit_message>
remove comments from listnodes
</commit_message>
<xml_diff>
--- a/testdata/excel2json/new_excel2json_files/lists/lists.xlsx
+++ b/testdata/excel2json/new_excel2json_files/lists/lists.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/dsp-tools/testdata/excel2json/new_excel2json_files/lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B547241A-2B3B-D849-94AB-BF1CC8515DC0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72062300-DFE3-494F-A0B7-2BC4BCC6AD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1140" yWindow="760" windowWidth="28860" windowHeight="20480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="list 1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="45">
   <si>
     <t>ID (optional)</t>
   </si>
@@ -156,6 +156,12 @@
   </si>
   <si>
     <t>List 2</t>
+  </si>
+  <si>
+    <t>List 3</t>
+  </si>
+  <si>
+    <t>Liste 2</t>
   </si>
 </sst>
 </file>
@@ -1808,7 +1814,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1831,19 +1837,19 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>2</v>
+      <c r="B2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
+      <c r="B3" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>44</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>3</v>
@@ -1872,7 +1878,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="182" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1887,12 +1893,12 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>3</v>
@@ -1900,7 +1906,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>11</v>
@@ -1908,7 +1914,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>17</v>
@@ -1916,7 +1922,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
test(excel2json): add integration test for new-lists (#1092)
</commit_message>
<xml_diff>
--- a/testdata/excel2json/new_excel2json_files/lists/lists.xlsx
+++ b/testdata/excel2json/new_excel2json_files/lists/lists.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/noraammann/Documents/Cloned_GitHub/dsp-tools/testdata/excel2json/new_excel2json_files/lists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72062300-DFE3-494F-A0B7-2BC4BCC6AD57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63A7D2EA-CAB3-7444-A1B8-81DB985D61D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="760" windowWidth="28860" windowHeight="20480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1140" yWindow="760" windowWidth="17480" windowHeight="20480" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="list 1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="33">
   <si>
     <t>ID (optional)</t>
   </si>
@@ -86,30 +85,6 @@
     <t>Knoten 3</t>
   </si>
   <si>
-    <t>Node 3.1</t>
-  </si>
-  <si>
-    <t>Knoten 3.1</t>
-  </si>
-  <si>
-    <t>Node 3.1.1</t>
-  </si>
-  <si>
-    <t>Knoten 3.1.1</t>
-  </si>
-  <si>
-    <t>Node 3.1.2</t>
-  </si>
-  <si>
-    <t>Knoten 3.1.2</t>
-  </si>
-  <si>
-    <t>Node 3.2</t>
-  </si>
-  <si>
-    <t>Knoten 3.2</t>
-  </si>
-  <si>
     <t>en_list</t>
   </si>
   <si>
@@ -134,21 +109,12 @@
     <t>de_3</t>
   </si>
   <si>
-    <t>Node 4</t>
-  </si>
-  <si>
-    <t>Knoten 4</t>
-  </si>
-  <si>
     <t>Knoten 1.1.2</t>
   </si>
   <si>
     <t>Knoten 1.1.1</t>
   </si>
   <si>
-    <t>custom_name_3-1-2</t>
-  </si>
-  <si>
     <t>Node 2.3</t>
   </si>
   <si>
@@ -158,21 +124,25 @@
     <t>List 2</t>
   </si>
   <si>
-    <t>List 3</t>
-  </si>
-  <si>
-    <t>Liste 2</t>
+    <t>subnode1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -238,11 +208,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
@@ -460,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I1000"/>
+  <dimension ref="A1:I995"/>
   <sheetViews>
     <sheetView zoomScale="142" workbookViewId="0">
-      <selection sqref="A1:E3"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -480,28 +451,28 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -572,7 +543,7 @@
         <v>8</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -601,7 +572,7 @@
         <v>10</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -677,10 +648,10 @@
         <v>12</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>40</v>
+        <v>29</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -699,115 +670,11 @@
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
     </row>
-    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
+    <row r="12" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="13" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="14" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="15" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="16" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="19" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1787,13 +1654,8 @@
     <row r="993" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="994" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="995" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="996" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="997" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="998" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="999" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
+  <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="A1">
     <cfRule type="colorScale" priority="1">
       <colorScale>
@@ -1811,125 +1673,71 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55FE4E04-8CBA-234A-8289-A15D83F3CCCF}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>44</v>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="5" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="1" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>4</v>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="A1">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FF57BB8A"/>
-        <color rgb="FFFFFFFF"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B8850B1-327B-5F47-B231-66A2329E5DA1}">
-  <dimension ref="A1:B6"/>
-  <sheetViews>
-    <sheetView zoomScale="182" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="5" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="6" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>